<commit_message>
Evolucion estructural de snedds  durante la digestion en tamaño y pdi con su tabla de analisis.
</commit_message>
<xml_diff>
--- a/Datos generales digestion.xlsx
+++ b/Datos generales digestion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heber\Desktop\proyecto 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EED451-F205-452F-8B90-3647F3EC673A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54C31A1-4364-4C9D-ACE9-2664A997856D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A64F9E11-6710-4C33-9930-3773814F4B53}"/>
   </bookViews>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3552EE2-2AF4-42CD-8CD2-7ADA7165F0C2}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,7 +826,7 @@
         <v>29.18</v>
       </c>
       <c r="I7" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.28899999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -855,7 +855,7 @@
         <v>25.42</v>
       </c>
       <c r="I8" s="3">
-        <v>0.16</v>
+        <v>0.161</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1029,7 +1029,7 @@
         <v>28.85</v>
       </c>
       <c r="I14" s="3">
-        <v>0.12</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1087,7 +1087,7 @@
         <v>25.83</v>
       </c>
       <c r="I16" s="3">
-        <v>0.15</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1145,7 +1145,7 @@
         <v>25.74</v>
       </c>
       <c r="I18" s="3">
-        <v>0.18</v>
+        <v>0.18099999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1319,7 +1319,7 @@
         <v>26.58</v>
       </c>
       <c r="I24" s="3">
-        <v>0.17</v>
+        <v>0.17899999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1493,7 +1493,7 @@
         <v>43.8</v>
       </c>
       <c r="I30" s="3">
-        <v>9.6000000000000002E-2</v>
+        <v>0.19600000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>